<commit_message>
imp price reduced to activate export
</commit_message>
<xml_diff>
--- a/VT_REG_PRI_V01.xlsx
+++ b/VT_REG_PRI_V01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr showObjects="placeholders" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda\Veda_models\Demo_models\DemoS_001\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda\Veda_models\DemoS_001\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B20BFD8-338A-4B58-A955-40D33E7C654B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB66CADA-42A3-4D23-AE93-29FAD2EDD18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="901" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="12735" tabRatio="901" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EnergyBalance" sheetId="133" r:id="rId1"/>
@@ -2044,9 +2044,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="General_)"/>
-    <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="General_)"/>
+    <numFmt numFmtId="166" formatCode="\Te\x\t"/>
   </numFmts>
   <fonts count="27" x14ac:knownFonts="1">
     <font>
@@ -2508,7 +2508,7 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2525,7 +2525,7 @@
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -2625,7 +2625,7 @@
     <xf numFmtId="1" fontId="15" fillId="6" borderId="9" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="5" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="6" borderId="5" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -2635,19 +2635,19 @@
     <xf numFmtId="1" fontId="15" fillId="6" borderId="14" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="13" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="13" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="14" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="14" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="14" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="14" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -2687,13 +2687,13 @@
     <xf numFmtId="1" fontId="15" fillId="6" borderId="15" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2716,27 +2716,27 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="20" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="20" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="20" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5142,7 +5142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -5208,8 +5208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5753,7 +5753,7 @@
       <c r="F16" s="12"/>
       <c r="G16" s="11"/>
       <c r="H16" s="68">
-        <v>2.75</v>
+        <v>2.7</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
@@ -6034,7 +6034,7 @@
   <dimension ref="B1:T28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6608,7 +6608,7 @@
   <dimension ref="B1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>